<commit_message>
formularios de emprendimiento v1
</commit_message>
<xml_diff>
--- a/Formatos CEIDEUL.xlsx
+++ b/Formatos CEIDEUL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JOHN\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\proyecto_tesis_v2\proyecto_tesis_v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{782721ED-2673-40D6-AAA5-590E35CCB7B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5AD4FB-D468-4905-99A1-C4F66E547E23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FORMATOS CEIDEUL" sheetId="1" r:id="rId1"/>
@@ -391,7 +391,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -439,8 +439,22 @@
       <name val="Corbel"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -457,6 +471,16 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -567,11 +591,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -628,6 +654,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -637,15 +669,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Bueno" xfId="2" builtinId="26"/>
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Incorrecto" xfId="3" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
@@ -12395,10 +12432,10 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C38" sqref="C38"/>
+      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12413,13 +12450,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="21" t="s">
+      <c r="A1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="21"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" spans="1:6" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
@@ -12701,7 +12738,7 @@
       <c r="A19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="25" t="s">
         <v>4</v>
       </c>
       <c r="C19" s="9" t="s">
@@ -12717,7 +12754,7 @@
       <c r="A20" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="27" t="s">
         <v>4</v>
       </c>
       <c r="C20" s="9" t="s">
@@ -12733,10 +12770,10 @@
       <c r="A21" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="24" t="s">
+      <c r="C21" s="21" t="s">
         <v>11</v>
       </c>
       <c r="D21" s="2"/>
@@ -12749,7 +12786,7 @@
       <c r="A22" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="27" t="s">
         <v>4</v>
       </c>
       <c r="C22" s="9" t="s">
@@ -12765,7 +12802,7 @@
       <c r="A23" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="25" t="s">
         <v>4</v>
       </c>
       <c r="C23" s="9" t="s">
@@ -12781,7 +12818,7 @@
       <c r="A24" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="26" t="s">
         <v>4</v>
       </c>
       <c r="C24" s="10" t="s">
@@ -12797,10 +12834,10 @@
       <c r="A25" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="23" t="s">
+      <c r="C25" s="20" t="s">
         <v>66</v>
       </c>
       <c r="D25" s="2"/>
@@ -12813,7 +12850,7 @@
       <c r="A26" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="26" t="s">
         <v>4</v>
       </c>
       <c r="C26" s="11" t="s">
@@ -12829,7 +12866,7 @@
       <c r="A27" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="26" t="s">
         <v>4</v>
       </c>
       <c r="C27" s="11" t="s">
@@ -12880,7 +12917,7 @@
       <c r="B30" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C30" s="23" t="s">
+      <c r="C30" s="20" t="s">
         <v>22</v>
       </c>
       <c r="D30" s="2"/>
@@ -12992,7 +13029,7 @@
       <c r="B37" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C37" s="23" t="s">
+      <c r="C37" s="20" t="s">
         <v>43</v>
       </c>
       <c r="D37" s="2"/>
@@ -13008,7 +13045,7 @@
       <c r="B38" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="23" t="s">
+      <c r="C38" s="20" t="s">
         <v>45</v>
       </c>
       <c r="D38" s="2"/>

</xml_diff>

<commit_message>
formatos de meprendimiento y proyeccion social
</commit_message>
<xml_diff>
--- a/Formatos CEIDEUL.xlsx
+++ b/Formatos CEIDEUL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\proyecto_tesis_v2\proyecto_tesis_v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5AD4FB-D468-4905-99A1-C4F66E547E23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0636DB17-B805-4372-A68C-9F670CB26ED2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -391,7 +391,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -446,15 +446,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -476,11 +469,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -591,13 +579,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -660,6 +647,9 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -669,20 +659,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="3">
     <cellStyle name="Bueno" xfId="2" builtinId="26"/>
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
-    <cellStyle name="Incorrecto" xfId="3" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
@@ -12435,7 +12418,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
+      <selection pane="bottomRight" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12450,13 +12433,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="23" t="s">
+      <c r="A1" s="23"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="23"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="24"/>
     </row>
     <row r="2" spans="1:6" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
@@ -12738,7 +12721,7 @@
       <c r="A19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="22" t="s">
         <v>4</v>
       </c>
       <c r="C19" s="9" t="s">
@@ -12754,7 +12737,7 @@
       <c r="A20" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="22" t="s">
         <v>4</v>
       </c>
       <c r="C20" s="9" t="s">
@@ -12770,7 +12753,7 @@
       <c r="A21" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="22" t="s">
         <v>4</v>
       </c>
       <c r="C21" s="21" t="s">
@@ -12786,7 +12769,7 @@
       <c r="A22" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B22" s="27" t="s">
+      <c r="B22" s="22" t="s">
         <v>4</v>
       </c>
       <c r="C22" s="9" t="s">
@@ -12802,7 +12785,7 @@
       <c r="A23" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="22" t="s">
         <v>4</v>
       </c>
       <c r="C23" s="9" t="s">

</xml_diff>

<commit_message>
MAS FORMS y excepcion a forms de volver a repetir
</commit_message>
<xml_diff>
--- a/Formatos CEIDEUL.xlsx
+++ b/Formatos CEIDEUL.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\proyecto_tesis_v2\proyecto_tesis_v2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Proyecto_Tesis_V2\proyecto_tesis_v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0636DB17-B805-4372-A68C-9F670CB26ED2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="FORMATOS CEIDEUL" sheetId="1" r:id="rId1"/>
@@ -390,7 +389,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -447,7 +446,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -469,6 +468,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -584,7 +589,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -650,6 +655,9 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -659,7 +667,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -12132,18 +12140,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A2:F38" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6">
-  <autoFilter ref="A2:F38" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:F38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A2:F38" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6">
+  <autoFilter ref="A2:F38"/>
+  <sortState ref="A3:F38">
     <sortCondition ref="A2:A40"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="CODIGO" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="AREA" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="FORMATO" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="EDITAR" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="PDF" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="LINK GOOGLE" dataDxfId="0"/>
+    <tableColumn id="1" name="CODIGO" dataDxfId="5"/>
+    <tableColumn id="2" name="AREA" dataDxfId="4"/>
+    <tableColumn id="3" name="FORMATO" dataDxfId="3"/>
+    <tableColumn id="4" name="EDITAR" dataDxfId="2"/>
+    <tableColumn id="5" name="PDF" dataDxfId="1"/>
+    <tableColumn id="6" name="LINK GOOGLE" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -12411,14 +12419,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomRight" activeCell="B32" sqref="B32:C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12433,13 +12441,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23"/>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24" t="s">
+      <c r="A1" s="24"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="24"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="25"/>
     </row>
     <row r="2" spans="1:6" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
@@ -12801,7 +12809,7 @@
       <c r="A24" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="23" t="s">
         <v>4</v>
       </c>
       <c r="C24" s="10" t="s">
@@ -12817,7 +12825,7 @@
       <c r="A25" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="23" t="s">
         <v>4</v>
       </c>
       <c r="C25" s="20" t="s">
@@ -12833,7 +12841,7 @@
       <c r="A26" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B26" s="26" t="s">
+      <c r="B26" s="23" t="s">
         <v>4</v>
       </c>
       <c r="C26" s="11" t="s">
@@ -12849,7 +12857,7 @@
       <c r="A27" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B27" s="26" t="s">
+      <c r="B27" s="23" t="s">
         <v>4</v>
       </c>
       <c r="C27" s="11" t="s">
@@ -12865,7 +12873,7 @@
       <c r="A28" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="27" t="s">
         <v>9</v>
       </c>
       <c r="C28" s="11" t="s">
@@ -12881,7 +12889,7 @@
       <c r="A29" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="27" t="s">
         <v>9</v>
       </c>
       <c r="C29" s="11" t="s">
@@ -12897,7 +12905,7 @@
       <c r="A30" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="27" t="s">
         <v>9</v>
       </c>
       <c r="C30" s="20" t="s">
@@ -12913,7 +12921,7 @@
       <c r="A31" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="27" t="s">
         <v>9</v>
       </c>
       <c r="C31" s="11" t="s">
@@ -13043,42 +13051,42 @@
     <mergeCell ref="C1:E1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="F4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="F5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="F6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="F7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="F8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="F9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="F10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="F11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="F12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="F13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="F14" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="F15" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="F16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="F17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="F18" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="F19" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="F20" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="F21" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="F22" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="F23" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="F24" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="F25" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="F26" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="F27" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="F28" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="F29" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="F30" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="F31" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="F32" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="F33" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="F34" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="F35" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="F36" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="F37" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="F38" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="F3" r:id="rId1"/>
+    <hyperlink ref="F4" r:id="rId2"/>
+    <hyperlink ref="F5" r:id="rId3"/>
+    <hyperlink ref="F6" r:id="rId4"/>
+    <hyperlink ref="F7" r:id="rId5"/>
+    <hyperlink ref="F8" r:id="rId6"/>
+    <hyperlink ref="F9" r:id="rId7"/>
+    <hyperlink ref="F10" r:id="rId8"/>
+    <hyperlink ref="F11" r:id="rId9"/>
+    <hyperlink ref="F12" r:id="rId10"/>
+    <hyperlink ref="F13" r:id="rId11"/>
+    <hyperlink ref="F14" r:id="rId12"/>
+    <hyperlink ref="F15" r:id="rId13"/>
+    <hyperlink ref="F16" r:id="rId14"/>
+    <hyperlink ref="F17" r:id="rId15"/>
+    <hyperlink ref="F18" r:id="rId16"/>
+    <hyperlink ref="F19" r:id="rId17"/>
+    <hyperlink ref="F20" r:id="rId18"/>
+    <hyperlink ref="F21" r:id="rId19"/>
+    <hyperlink ref="F22" r:id="rId20"/>
+    <hyperlink ref="F23" r:id="rId21"/>
+    <hyperlink ref="F24" r:id="rId22"/>
+    <hyperlink ref="F25" r:id="rId23"/>
+    <hyperlink ref="F26" r:id="rId24"/>
+    <hyperlink ref="F27" r:id="rId25"/>
+    <hyperlink ref="F28" r:id="rId26"/>
+    <hyperlink ref="F29" r:id="rId27"/>
+    <hyperlink ref="F30" r:id="rId28"/>
+    <hyperlink ref="F31" r:id="rId29"/>
+    <hyperlink ref="F32" r:id="rId30"/>
+    <hyperlink ref="F33" r:id="rId31"/>
+    <hyperlink ref="F34" r:id="rId32"/>
+    <hyperlink ref="F35" r:id="rId33"/>
+    <hyperlink ref="F36" r:id="rId34"/>
+    <hyperlink ref="F37" r:id="rId35"/>
+    <hyperlink ref="F38" r:id="rId36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId37"/>

</xml_diff>